<commit_message>
Updated List and temporary
Updated the excel-file
Updated the temporary-file with overviw
</commit_message>
<xml_diff>
--- a/Traits_Mod.xlsx
+++ b/Traits_Mod.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17766"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shane\Documents\GitHub\TheCK2Project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="106">
   <si>
     <t>ID</t>
   </si>
@@ -169,12 +164,6 @@
   </si>
   <si>
     <t>Albino</t>
-  </si>
-  <si>
-    <t>15% Inherit Chance</t>
-  </si>
-  <si>
-    <t>20% Inherit Chance</t>
   </si>
   <si>
     <t>albino</t>
@@ -204,9 +193,6 @@
 +100 Same Trait</t>
   </si>
   <si>
-    <t>5% Inherit Chance</t>
-  </si>
-  <si>
     <t>Congenital</t>
   </si>
   <si>
@@ -229,14 +215,7 @@
     <t>Opposite of Dwarf.</t>
   </si>
   <si>
-    <t>20% Inherit Chance
-+10.0% Moral</t>
-  </si>
-  <si>
     <t>downsyndrome</t>
-  </si>
-  <si>
-    <t>Needs Regent</t>
   </si>
   <si>
     <t>Racist</t>
@@ -264,9 +243,6 @@
     <t>+20.00</t>
   </si>
   <si>
-    <t>Available through event.</t>
-  </si>
-  <si>
     <t>Intelligent</t>
   </si>
   <si>
@@ -277,12 +253,6 @@
   </si>
   <si>
     <t>+10 General</t>
-  </si>
-  <si>
-    <t>Opposite of Slow</t>
-  </si>
-  <si>
-    <t>100 rationality</t>
   </si>
   <si>
     <t>+1000%</t>
@@ -309,12 +279,92 @@
   <si>
     <t>-10 Attraction
 -5 General</t>
+  </si>
+  <si>
+    <t>Opposite of Funny.</t>
+  </si>
+  <si>
+    <t>Opposite of Cringey.</t>
+  </si>
+  <si>
+    <t>Needs Regent.</t>
+  </si>
+  <si>
+    <t>-30 Rationality</t>
+  </si>
+  <si>
+    <t>Equalist</t>
+  </si>
+  <si>
+    <t>equalist</t>
+  </si>
+  <si>
+    <t>Opposite of Equalist.</t>
+  </si>
+  <si>
+    <t>Available through event. Immortal.</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Sympathy for every Religion.</t>
+  </si>
+  <si>
+    <t>Rationality</t>
+  </si>
+  <si>
+    <t>+100 Rationality</t>
+  </si>
+  <si>
+    <t>Opposite of Slow, Imbecile and Genius.</t>
+  </si>
+  <si>
+    <t>Opposite of Racist, Zealous.</t>
+  </si>
+  <si>
+    <t>15% Inherit Chance. 
+30 % Both Parents
+1% Birth</t>
+  </si>
+  <si>
+    <t>25% Inherit Chance
+50% Both Parents
+Inbred.</t>
+  </si>
+  <si>
+    <t>5% Inherit Chance
+10% Both Parents
+2% Birth</t>
+  </si>
+  <si>
+    <t>20% Inherit Chance
+40% Both Parents
+1% Birth
++10.0% Moral</t>
+  </si>
+  <si>
+    <t>10% Inherit Chance.
+30% Both Parents
+Enables the Clever Ambush combat tactic.</t>
+  </si>
+  <si>
+    <t>+15 Rationality</t>
+  </si>
+  <si>
+    <t>-10 Ambition</t>
+  </si>
+  <si>
+    <t>+10 Ambition</t>
+  </si>
+  <si>
+    <t>Not random</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -384,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -398,6 +448,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -417,9 +470,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -457,9 +510,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -492,26 +545,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -544,26 +580,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -737,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P30"/>
+  <dimension ref="B1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,12 +770,13 @@
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="12" max="12" width="22.140625" style="4" customWidth="1"/>
     <col min="13" max="13" width="24.140625" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" customWidth="1"/>
-    <col min="15" max="15" width="18.5703125" customWidth="1"/>
+    <col min="14" max="14" width="25.28515625" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" customWidth="1"/>
+    <col min="16" max="16" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>0</v>
@@ -795,13 +815,16 @@
         <v>9</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="P2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:17" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
@@ -809,7 +832,7 @@
         <v>300</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>14</v>
@@ -832,13 +855,16 @@
       </c>
       <c r="N3" s="3"/>
       <c r="O3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="P3" s="2">
+        <v>103</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q3" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:17" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
@@ -873,13 +899,16 @@
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="P4" s="2">
+        <v>104</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:17" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>46</v>
       </c>
@@ -902,15 +931,18 @@
         <v>34</v>
       </c>
       <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="P5" s="2">
+      <c r="N5" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q5" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:17" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
@@ -935,15 +967,18 @@
         <v>33</v>
       </c>
       <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="P6" s="2">
+      <c r="N6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q6" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
@@ -966,15 +1001,18 @@
         <v>33</v>
       </c>
       <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="P7" s="2">
+      <c r="N7" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q7" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
@@ -997,15 +1035,18 @@
         <v>33</v>
       </c>
       <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="P8" s="2">
+      <c r="N8" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q8" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>31</v>
       </c>
@@ -1028,23 +1069,26 @@
         <v>33</v>
       </c>
       <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="P9" s="2">
+      <c r="N9" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q9" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C10" s="2">
         <v>307</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>13</v>
@@ -1060,18 +1104,23 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="O10" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="P10" s="2">
+      <c r="P10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q10" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:17" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>35</v>
       </c>
@@ -1079,7 +1128,7 @@
         <v>308</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>39</v>
@@ -1091,18 +1140,21 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="M11" s="3"/>
+        <v>82</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="N11" s="3"/>
-      <c r="O11" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="P11" s="2">
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O11" s="3"/>
+      <c r="P11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>36</v>
       </c>
@@ -1126,18 +1178,21 @@
         <v>38</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="M12" s="3"/>
+        <v>49</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="N12" s="3"/>
-      <c r="O12" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="P12" s="2">
+      <c r="O12" s="3"/>
+      <c r="P12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q12" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="2:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:17" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>40</v>
       </c>
@@ -1145,7 +1200,7 @@
         <v>310</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>15</v>
@@ -1165,20 +1220,21 @@
         <v>41</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="P13" s="2">
+        <v>97</v>
+      </c>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q13" s="2">
         <v>-4</v>
       </c>
     </row>
-    <row r="14" spans="2:16" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:17" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>42</v>
       </c>
@@ -1186,7 +1242,7 @@
         <v>311</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>44</v>
@@ -1208,22 +1264,23 @@
         <v>45</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="P14" s="2">
+        <v>98</v>
+      </c>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q14" s="2">
         <v>-35</v>
       </c>
     </row>
-    <row r="15" spans="2:16" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:17" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>47</v>
       </c>
@@ -1231,7 +1288,7 @@
         <v>312</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>15</v>
@@ -1245,34 +1302,35 @@
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L15" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="M15" s="3"/>
       <c r="N15" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="O15" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="P15" s="2">
+      <c r="Q15" s="2">
         <v>-20</v>
       </c>
     </row>
-    <row r="16" spans="2:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:17" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C16" s="2">
         <v>313</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>13</v>
@@ -1288,30 +1346,31 @@
         <v>38</v>
       </c>
       <c r="L16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="P16" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="C17" s="2">
         <v>314</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>15</v>
@@ -1323,125 +1382,153 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="M17" s="3"/>
+        <v>65</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="N17" s="3"/>
-      <c r="O17" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="P17" s="2">
+      <c r="O17" s="3"/>
+      <c r="P17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q17" s="2">
         <v>-4</v>
       </c>
     </row>
-    <row r="18" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:17" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C18" s="2">
         <v>315</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="J18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K18" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="K18" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="L18" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>82</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="N18" s="3"/>
       <c r="O18" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="P18" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q18" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C19" s="2">
         <v>316</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="P19" s="2">
+        <v>102</v>
+      </c>
+      <c r="P19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q19" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="1"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="3"/>
+    <row r="20" spans="2:17" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="2">
+        <v>317</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="G20" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="I20" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
+      <c r="M20" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="O20" s="3"/>
-      <c r="P20" s="2"/>
-    </row>
-    <row r="21" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1456,9 +1543,10 @@
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
-      <c r="P21" s="2"/>
-    </row>
-    <row r="22" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P21" s="3"/>
+      <c r="Q21" s="2"/>
+    </row>
+    <row r="22" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1473,9 +1561,10 @@
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
-      <c r="P22" s="2"/>
-    </row>
-    <row r="23" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P22" s="3"/>
+      <c r="Q22" s="2"/>
+    </row>
+    <row r="23" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1490,9 +1579,10 @@
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
-      <c r="P23" s="2"/>
-    </row>
-    <row r="24" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P23" s="3"/>
+      <c r="Q23" s="2"/>
+    </row>
+    <row r="24" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1507,9 +1597,10 @@
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
-      <c r="P24" s="2"/>
-    </row>
-    <row r="25" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P24" s="3"/>
+      <c r="Q24" s="2"/>
+    </row>
+    <row r="25" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1524,9 +1615,10 @@
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
-      <c r="P25" s="2"/>
-    </row>
-    <row r="26" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P25" s="3"/>
+      <c r="Q25" s="2"/>
+    </row>
+    <row r="26" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1541,9 +1633,10 @@
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
-      <c r="P26" s="2"/>
-    </row>
-    <row r="27" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P26" s="3"/>
+      <c r="Q26" s="2"/>
+    </row>
+    <row r="27" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1558,9 +1651,10 @@
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
-      <c r="P27" s="2"/>
-    </row>
-    <row r="28" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P27" s="3"/>
+      <c r="Q27" s="2"/>
+    </row>
+    <row r="28" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1575,9 +1669,10 @@
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
-      <c r="P28" s="2"/>
-    </row>
-    <row r="29" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P28" s="3"/>
+      <c r="Q28" s="2"/>
+    </row>
+    <row r="29" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1592,9 +1687,10 @@
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
-      <c r="P29" s="2"/>
-    </row>
-    <row r="30" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P29" s="3"/>
+      <c r="Q29" s="2"/>
+    </row>
+    <row r="30" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1609,7 +1705,8 @@
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
-      <c r="P30" s="2"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>